<commit_message>
exaggerating differences for visual effect
</commit_message>
<xml_diff>
--- a/data/fake_rasts.xlsx
+++ b/data/fake_rasts.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohara/github/fig_for_spp_chi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0864F5EC-FBD2-0C4F-B32B-E58F8C841F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7171840C-EF07-484C-A97A-EE8AF12C6073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25260" windowHeight="12260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="4820" windowWidth="25260" windowHeight="12260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spp1" sheetId="1" r:id="rId1"/>
     <sheet name="spp2" sheetId="2" r:id="rId2"/>
     <sheet name="spp3" sheetId="3" r:id="rId3"/>
     <sheet name="spp4" sheetId="4" r:id="rId4"/>
-    <sheet name="str1" sheetId="5" r:id="rId5"/>
-    <sheet name="str2" sheetId="6" r:id="rId6"/>
-    <sheet name="str3" sheetId="7" r:id="rId7"/>
+    <sheet name="str1" sheetId="7" r:id="rId5"/>
+    <sheet name="str3" sheetId="5" r:id="rId6"/>
+    <sheet name="str2" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -361,8 +361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -521,10 +521,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -553,10 +553,10 @@
         <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -585,10 +585,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -617,10 +617,10 @@
         <v>1</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -652,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -684,7 +684,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1741,6 +1741,392 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H1" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I1" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:K10">
+    <sortCondition descending="1" ref="G1:G10"/>
+  </sortState>
+  <conditionalFormatting sqref="G1:J4">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color theme="4" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:J10">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color theme="4" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:F10">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color theme="4" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:J10">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -2068,359 +2454,6 @@
       </c>
       <c r="J10" s="1">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:J10">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <color theme="4" tint="-0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1">
-        <v>0</v>
-      </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -2447,27 +2480,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="B1" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1">
         <v>0</v>
@@ -2490,19 +2523,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="C2" s="1">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -2528,16 +2561,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -2554,22 +2587,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F4" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -2578,135 +2611,135 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D5" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H5" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="1">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="I6" s="1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J6" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F7" s="1">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G7" s="1">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I7" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="B8" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H8" s="1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="I8" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
@@ -2714,31 +2747,31 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
@@ -2746,16 +2779,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -2764,29 +2797,19 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:F10">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <color theme="4" tint="-0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A1:J10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -2796,18 +2819,6 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:J4">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <color theme="4" tint="-0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:J10">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>